<commit_message>
começando treinadores da arena de Alana
</commit_message>
<xml_diff>
--- a/Assets/Documentos/Elementos de GDD.xlsx
+++ b/Assets/Documentos/Elementos de GDD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FluxoDeJogo" sheetId="1" r:id="rId1"/>
@@ -714,7 +714,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -743,6 +743,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Ênfase1" xfId="3" builtinId="30"/>
@@ -1052,7 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1944,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,8 +1956,8 @@
       <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>29</v>
+      <c r="C3" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>56</v>
@@ -1963,8 +1965,8 @@
       <c r="F3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>35</v>
+      <c r="G3" s="14" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -2005,8 +2007,8 @@
       <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>35</v>
+      <c r="C6" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>59</v>
@@ -2096,8 +2098,8 @@
       <c r="F11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>29</v>
+      <c r="G11" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>